<commit_message>
feat: add statistics completed tasks
</commit_message>
<xml_diff>
--- a/src/data/Tasks.xlsx
+++ b/src/data/Tasks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Петр\petriken-2018Q3\rss-mentor-dashboard\src\_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Петр\Community-lab\mentor-dashboard\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -87,9 +87,6 @@
     <t>https://github.com/rolling-scopes-school/tasks/blob/2018-Q3/tasks/youtube.md</t>
   </si>
   <si>
-    <t>CodeJam "Scoreboard"</t>
-  </si>
-  <si>
     <t>https://github.com/rolling-scopes-school/tasks/blob/2018-Q3/tasks/codejam-scoreboard.md</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>https://github.com/rolling-scopes-school/tasks/blob/2018-Q3/tasks/presentation.md</t>
+  </si>
+  <si>
+    <t>Code Jam "Scoreboard"</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -554,7 +554,7 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>19</v>
@@ -576,10 +576,10 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
@@ -587,10 +587,10 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -598,10 +598,10 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -609,7 +609,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>

</xml_diff>